<commit_message>
Stor ändring av lager med koppling till firebase
</commit_message>
<xml_diff>
--- a/bilder/01 - Produktlista.xlsx
+++ b/bilder/01 - Produktlista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosse\Desktop\TechZon\TechZon_Github\bilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAE0FE1-A6F0-44C4-AB06-31DA2EAA147D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C542FD6A-7EC2-4FD2-BD05-404E3651652F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>Kod</t>
   </si>
@@ -175,12 +175,6 @@
     <t>Kommentar</t>
   </si>
   <si>
-    <t>Iphone 16</t>
-  </si>
-  <si>
-    <t>Tre olika färger</t>
-  </si>
-  <si>
     <t>Samsung 24 Ultra</t>
   </si>
   <si>
@@ -212,6 +206,21 @@
   </si>
   <si>
     <t>5D glas skärmskydd Samsung Galaxy S24 Ultra</t>
+  </si>
+  <si>
+    <t>Iphone 15 Pro</t>
+  </si>
+  <si>
+    <t>Svart XX</t>
+  </si>
+  <si>
+    <t>Svart XY</t>
+  </si>
+  <si>
+    <t>Vitt YY</t>
+  </si>
+  <si>
+    <t>Guld YX</t>
   </si>
 </sst>
 </file>
@@ -650,7 +659,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,13 +698,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -703,10 +712,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -714,25 +726,49 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -807,7 +843,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -818,7 +854,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -829,7 +865,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -924,7 +960,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -935,7 +971,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -946,7 +982,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1041,7 +1077,7 @@
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1052,7 +1088,7 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1063,7 +1099,7 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>5</v>

</xml_diff>